<commit_message>
Implimented reading from Word Storage.
</commit_message>
<xml_diff>
--- a/Kanji Storage.xlsx
+++ b/Kanji Storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\Japanese Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E2C7F0-A835-4374-A595-FD34D6A159F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553E5A31-B8FF-4B2C-BFFB-769F1E8F503A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="16080" windowWidth="19440" windowHeight="10590" xr2:uid="{D6FF4FC2-0135-406D-A64E-1610F306DCDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6FF4FC2-0135-406D-A64E-1610F306DCDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3897,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF80FB1D-2E71-48B9-B9D5-5987A57EBCD1}">
   <dimension ref="A1:N229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>